<commit_message>
Updated verified status of polarized caps table to tralse, as the library is yet to be used but seems to work.
</commit_message>
<xml_diff>
--- a/To Add v2/00 Things To Add.xlsx
+++ b/To Add v2/00 Things To Add.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Danakil_KiCad_DB\To Add v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215782B9-13BE-4687-886F-9994584AD85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695D9F58-E80D-4E8C-AC6A-2D6DFDE88FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3470" yWindow="2200" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="218">
   <si>
     <t>Table Name</t>
   </si>
@@ -846,7 +846,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -921,7 +921,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1347,8 +1346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AE151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1694,14 +1693,14 @@
       <c r="S12" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="T12" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="U12" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="V12" t="b">
-        <v>0</v>
+      <c r="T12" t="b">
+        <v>1</v>
+      </c>
+      <c r="U12" t="b">
+        <v>1</v>
+      </c>
+      <c r="V12" t="s">
+        <v>184</v>
       </c>
       <c r="W12">
         <v>4</v>
@@ -2163,22 +2162,22 @@
       <c r="P18" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="Q18" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="R18" s="30" t="b">
+      <c r="Q18" t="b">
+        <v>0</v>
+      </c>
+      <c r="R18" t="b">
         <v>0</v>
       </c>
       <c r="S18" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="T18" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="U18" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="V18" s="30" t="b">
+      <c r="T18" t="b">
+        <v>0</v>
+      </c>
+      <c r="U18" t="b">
+        <v>0</v>
+      </c>
+      <c r="V18" t="b">
         <v>0</v>
       </c>
       <c r="W18">
@@ -2666,7 +2665,7 @@
       <c r="I25" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="J25" s="30" t="s">
+      <c r="J25" t="s">
         <v>59</v>
       </c>
       <c r="P25" s="6" t="b">
@@ -8224,22 +8223,22 @@
       <c r="P103" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="Q103" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="R103" s="30" t="b">
+      <c r="Q103" t="b">
+        <v>0</v>
+      </c>
+      <c r="R103" t="b">
         <v>0</v>
       </c>
       <c r="S103" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="T103" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="U103" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="V103" s="30" t="b">
+      <c r="T103" t="b">
+        <v>0</v>
+      </c>
+      <c r="U103" t="b">
+        <v>0</v>
+      </c>
+      <c r="V103" t="b">
         <v>0</v>
       </c>
       <c r="W103">
@@ -8295,22 +8294,22 @@
       <c r="P104" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="Q104" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="R104" s="30" t="b">
+      <c r="Q104" t="b">
+        <v>0</v>
+      </c>
+      <c r="R104" t="b">
         <v>0</v>
       </c>
       <c r="S104" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="T104" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="U104" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="V104" s="30" t="b">
+      <c r="T104" t="b">
+        <v>0</v>
+      </c>
+      <c r="U104" t="b">
+        <v>0</v>
+      </c>
+      <c r="V104" t="b">
         <v>0</v>
       </c>
       <c r="W104">
@@ -8363,22 +8362,22 @@
       <c r="P105" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="Q105" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="R105" s="30" t="b">
+      <c r="Q105" t="b">
+        <v>0</v>
+      </c>
+      <c r="R105" t="b">
         <v>0</v>
       </c>
       <c r="S105" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="T105" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="U105" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="V105" s="30" t="b">
+      <c r="T105" t="b">
+        <v>0</v>
+      </c>
+      <c r="U105" t="b">
+        <v>0</v>
+      </c>
+      <c r="V105" t="b">
         <v>0</v>
       </c>
       <c r="W105">
@@ -8425,28 +8424,28 @@
       <c r="I106" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="J106" s="30" t="s">
+      <c r="J106" t="s">
         <v>215</v>
       </c>
       <c r="P106" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="Q106" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="R106" s="30" t="b">
+      <c r="Q106" t="b">
+        <v>0</v>
+      </c>
+      <c r="R106" t="b">
         <v>0</v>
       </c>
       <c r="S106" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="T106" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="U106" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="V106" s="30" t="b">
+      <c r="T106" t="b">
+        <v>0</v>
+      </c>
+      <c r="U106" t="b">
+        <v>0</v>
+      </c>
+      <c r="V106" t="b">
         <v>0</v>
       </c>
       <c r="W106">
@@ -8502,22 +8501,22 @@
       <c r="P107" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="Q107" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="R107" s="30" t="b">
+      <c r="Q107" t="b">
+        <v>0</v>
+      </c>
+      <c r="R107" t="b">
         <v>0</v>
       </c>
       <c r="S107" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="T107" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="U107" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="V107" s="30" t="b">
+      <c r="T107" t="b">
+        <v>0</v>
+      </c>
+      <c r="U107" t="b">
+        <v>0</v>
+      </c>
+      <c r="V107" t="b">
         <v>0</v>
       </c>
       <c r="W107">
@@ -8573,22 +8572,22 @@
       <c r="P108" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="Q108" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="R108" s="30" t="b">
+      <c r="Q108" t="b">
+        <v>0</v>
+      </c>
+      <c r="R108" t="b">
         <v>0</v>
       </c>
       <c r="S108" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="T108" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="U108" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="V108" s="30" t="b">
+      <c r="T108" t="b">
+        <v>0</v>
+      </c>
+      <c r="U108" t="b">
+        <v>0</v>
+      </c>
+      <c r="V108" t="b">
         <v>0</v>
       </c>
       <c r="W108">
@@ -9141,10 +9140,10 @@
       <c r="S116" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="T116" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="U116" s="30" t="b">
+      <c r="T116" t="b">
+        <v>1</v>
+      </c>
+      <c r="U116" t="b">
         <v>1</v>
       </c>
       <c r="V116" t="b">
@@ -9546,22 +9545,22 @@
       <c r="P122" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="Q122" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="R122" s="30" t="b">
+      <c r="Q122" t="b">
+        <v>1</v>
+      </c>
+      <c r="R122" t="b">
         <v>1</v>
       </c>
       <c r="S122" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="T122" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="U122" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="V122" s="30" t="b">
+      <c r="T122" t="b">
+        <v>1</v>
+      </c>
+      <c r="U122" t="b">
+        <v>1</v>
+      </c>
+      <c r="V122" t="b">
         <v>1</v>
       </c>
       <c r="W122">
@@ -9614,22 +9613,22 @@
       <c r="P123" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="Q123" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="R123" s="30" t="b">
+      <c r="Q123" t="b">
+        <v>1</v>
+      </c>
+      <c r="R123" t="b">
         <v>1</v>
       </c>
       <c r="S123" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="T123" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="U123" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="V123" s="30" t="b">
+      <c r="T123" t="b">
+        <v>1</v>
+      </c>
+      <c r="U123" t="b">
+        <v>1</v>
+      </c>
+      <c r="V123" t="b">
         <v>1</v>
       </c>
       <c r="W123">
@@ -9682,22 +9681,22 @@
       <c r="P124" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="Q124" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="R124" s="30" t="b">
+      <c r="Q124" t="b">
+        <v>1</v>
+      </c>
+      <c r="R124" t="b">
         <v>1</v>
       </c>
       <c r="S124" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="T124" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="U124" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="V124" s="30" t="b">
+      <c r="T124" t="b">
+        <v>1</v>
+      </c>
+      <c r="U124" t="b">
+        <v>1</v>
+      </c>
+      <c r="V124" t="b">
         <v>1</v>
       </c>
       <c r="W124">
@@ -9969,22 +9968,22 @@
       <c r="P128" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="Q128" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="R128" s="30" t="b">
+      <c r="Q128" t="b">
+        <v>1</v>
+      </c>
+      <c r="R128" t="b">
         <v>1</v>
       </c>
       <c r="S128" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="T128" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="U128" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="V128" s="30" t="b">
+      <c r="T128" t="b">
+        <v>1</v>
+      </c>
+      <c r="U128" t="b">
+        <v>1</v>
+      </c>
+      <c r="V128" t="b">
         <v>1</v>
       </c>
       <c r="W128">
@@ -10043,22 +10042,22 @@
       <c r="P129" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="Q129" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="R129" s="30" t="b">
+      <c r="Q129" t="b">
+        <v>1</v>
+      </c>
+      <c r="R129" t="b">
         <v>1</v>
       </c>
       <c r="S129" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="T129" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="U129" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="V129" s="30" t="b">
+      <c r="T129" t="b">
+        <v>1</v>
+      </c>
+      <c r="U129" t="b">
+        <v>1</v>
+      </c>
+      <c r="V129" t="b">
         <v>1</v>
       </c>
       <c r="W129">
@@ -10114,22 +10113,22 @@
       <c r="P130" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="Q130" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="R130" s="30" t="b">
+      <c r="Q130" t="b">
+        <v>1</v>
+      </c>
+      <c r="R130" t="b">
         <v>1</v>
       </c>
       <c r="S130" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="T130" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="U130" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="V130" s="30" t="b">
+      <c r="T130" t="b">
+        <v>1</v>
+      </c>
+      <c r="U130" t="b">
+        <v>1</v>
+      </c>
+      <c r="V130" t="b">
         <v>1</v>
       </c>
       <c r="W130">
@@ -10185,22 +10184,22 @@
       <c r="P131" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="Q131" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="R131" s="30" t="b">
+      <c r="Q131" t="b">
+        <v>1</v>
+      </c>
+      <c r="R131" t="b">
         <v>1</v>
       </c>
       <c r="S131" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="T131" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="U131" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="V131" s="30" t="b">
+      <c r="T131" t="b">
+        <v>1</v>
+      </c>
+      <c r="U131" t="b">
+        <v>1</v>
+      </c>
+      <c r="V131" t="b">
         <v>1</v>
       </c>
       <c r="W131">
@@ -10250,22 +10249,22 @@
       <c r="P132" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="Q132" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="R132" s="30" t="b">
+      <c r="Q132" t="b">
+        <v>1</v>
+      </c>
+      <c r="R132" t="b">
         <v>1</v>
       </c>
       <c r="S132" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="T132" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="U132" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="V132" s="30" t="b">
+      <c r="T132" t="b">
+        <v>1</v>
+      </c>
+      <c r="U132" t="b">
+        <v>1</v>
+      </c>
+      <c r="V132" t="b">
         <v>1</v>
       </c>
       <c r="W132">
@@ -11217,7 +11216,7 @@
       <c r="I146" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="J146" s="30" t="s">
+      <c r="J146" t="s">
         <v>204</v>
       </c>
       <c r="P146" s="6" t="b">
@@ -11291,22 +11290,22 @@
       <c r="P147" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="Q147" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="R147" s="30" t="b">
+      <c r="Q147" t="b">
+        <v>1</v>
+      </c>
+      <c r="R147" t="b">
         <v>1</v>
       </c>
       <c r="S147" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="T147" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="U147" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="V147" s="30" t="b">
+      <c r="T147" t="b">
+        <v>1</v>
+      </c>
+      <c r="U147" t="b">
+        <v>1</v>
+      </c>
+      <c r="V147" t="b">
         <v>1</v>
       </c>
       <c r="W147">
@@ -11359,22 +11358,22 @@
       <c r="P148" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="Q148" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="R148" s="30" t="b">
+      <c r="Q148" t="b">
+        <v>1</v>
+      </c>
+      <c r="R148" t="b">
         <v>1</v>
       </c>
       <c r="S148" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="T148" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="U148" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="V148" s="30" t="b">
+      <c r="T148" t="b">
+        <v>1</v>
+      </c>
+      <c r="U148" t="b">
+        <v>1</v>
+      </c>
+      <c r="V148" t="b">
         <v>1</v>
       </c>
       <c r="W148">
@@ -11427,22 +11426,22 @@
       <c r="P149" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="Q149" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="R149" s="30" t="b">
+      <c r="Q149" t="b">
+        <v>1</v>
+      </c>
+      <c r="R149" t="b">
         <v>1</v>
       </c>
       <c r="S149" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="T149" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="U149" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="V149" s="30" t="b">
+      <c r="T149" t="b">
+        <v>1</v>
+      </c>
+      <c r="U149" t="b">
+        <v>1</v>
+      </c>
+      <c r="V149" t="b">
         <v>1</v>
       </c>
       <c r="W149">
@@ -11572,10 +11571,10 @@
       <c r="S151" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="T151" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="U151" s="30" t="b">
+      <c r="T151" t="b">
+        <v>1</v>
+      </c>
+      <c r="U151" t="b">
         <v>1</v>
       </c>
       <c r="V151" t="b">

</xml_diff>